<commit_message>
notes. only delay for now
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\5g-cop\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A25BDE-2239-4992-AEDF-F99B58879C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA079883-E9BF-414F-A695-293CC041FC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{398FC3E8-3646-4E76-9457-E32DE5631863}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{398FC3E8-3646-4E76-9457-E32DE5631863}"/>
   </bookViews>
   <sheets>
     <sheet name="delay" sheetId="1" r:id="rId1"/>
@@ -3571,7 +3571,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4420,7 +4419,7 @@
   <dimension ref="A1:BB17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE15" sqref="AE15"/>
+      <selection activeCell="BH26" sqref="BH26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5824,7 +5823,7 @@
         <v>32.724455686840692</v>
       </c>
       <c r="AJ12">
-        <f t="shared" ref="AI12:AL12" si="10">_xlfn.STDEV.P(AJ2:AJ11)</f>
+        <f t="shared" ref="AJ12:AL12" si="10">_xlfn.STDEV.P(AJ2:AJ11)</f>
         <v>4.6141087980237305</v>
       </c>
       <c r="AK12">
@@ -5987,7 +5986,7 @@
         <v>28.683723037615355</v>
       </c>
       <c r="AJ13">
-        <f t="shared" ref="AI13:AL13" si="15">_xlfn.CONFIDENCE.NORM($B$17,AJ12,5)</f>
+        <f t="shared" ref="AJ13:AL13" si="15">_xlfn.CONFIDENCE.NORM($B$17,AJ12,5)</f>
         <v>4.0443703661405159</v>
       </c>
       <c r="AK13">
@@ -6150,7 +6149,7 @@
         <v>1058.9000000000001</v>
       </c>
       <c r="AJ14">
-        <f t="shared" ref="AI14:AL14" si="22">AVERAGE(AJ2:AJ11)</f>
+        <f t="shared" ref="AJ14:AL14" si="22">AVERAGE(AJ2:AJ11)</f>
         <v>1600.1</v>
       </c>
       <c r="AK14">
@@ -6467,7 +6466,7 @@
         <v>491</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="C12:F12" si="0">_xlfn.STDEV.P(D2:D11)</f>
+        <f t="shared" ref="D12:F12" si="0">_xlfn.STDEV.P(D2:D11)</f>
         <v>47.345643939015126</v>
       </c>
       <c r="E12">
@@ -6544,10 +6543,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72F10BB-214C-4AE0-B137-46C905AF79B9}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6576,6 +6575,9 @@
       <c r="B2">
         <v>530</v>
       </c>
+      <c r="C2">
+        <v>520</v>
+      </c>
       <c r="D2">
         <v>1811</v>
       </c>
@@ -6591,7 +6593,7 @@
         <v>496</v>
       </c>
       <c r="C3">
-        <v>1161</v>
+        <v>496</v>
       </c>
       <c r="D3">
         <v>1838</v>
@@ -6608,7 +6610,7 @@
         <v>515</v>
       </c>
       <c r="C4">
-        <v>1145</v>
+        <v>495</v>
       </c>
       <c r="D4">
         <v>1824</v>
@@ -6625,7 +6627,7 @@
         <v>486</v>
       </c>
       <c r="C5">
-        <v>1254</v>
+        <v>496</v>
       </c>
       <c r="D5">
         <v>1929</v>
@@ -6642,7 +6644,7 @@
         <v>485</v>
       </c>
       <c r="C6">
-        <v>1271</v>
+        <v>489</v>
       </c>
       <c r="D6">
         <v>1932</v>
@@ -6659,7 +6661,7 @@
         <v>510</v>
       </c>
       <c r="C7">
-        <v>1157</v>
+        <v>494</v>
       </c>
       <c r="D7">
         <v>1806</v>
@@ -6676,7 +6678,7 @@
         <v>491</v>
       </c>
       <c r="C8">
-        <v>1142</v>
+        <v>496</v>
       </c>
       <c r="D8">
         <v>1847</v>
@@ -6693,7 +6695,7 @@
         <v>490</v>
       </c>
       <c r="C9">
-        <v>1146</v>
+        <v>490</v>
       </c>
       <c r="D9">
         <v>1799</v>
@@ -6710,7 +6712,7 @@
         <v>493</v>
       </c>
       <c r="C10">
-        <v>1148</v>
+        <v>489</v>
       </c>
       <c r="D10">
         <v>1814</v>
@@ -6727,7 +6729,7 @@
         <v>504</v>
       </c>
       <c r="C11">
-        <v>1205</v>
+        <v>495</v>
       </c>
       <c r="D11">
         <v>1803</v>
@@ -6744,12 +6746,12 @@
         <f>_xlfn.STDEV.P(B2:B11)</f>
         <v>13.813037319865606</v>
       </c>
-      <c r="C12">
-        <f t="shared" ref="C12:F12" si="0">_xlfn.STDEV.P(C2:C11)</f>
-        <v>47.272261069962227</v>
+      <c r="C12" t="e">
+        <f>_xlfn.STDEV.P(#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C12:E12" si="0">_xlfn.STDEV.P(D2:D11)</f>
         <v>47.345643939015126</v>
       </c>
       <c r="E12">
@@ -6765,9 +6767,9 @@
         <f>_xlfn.CONFIDENCE.NORM(B17,B12,5)</f>
         <v>12.107438564687733</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="e">
         <f>_xlfn.CONFIDENCE.NORM($B$17,C12,5)</f>
-        <v>41.435202371842706</v>
+        <v>#REF!</v>
       </c>
       <c r="D13">
         <f>_xlfn.CONFIDENCE.NORM($B$17,D12,5)</f>
@@ -6786,12 +6788,12 @@
         <f>AVERAGE(B2:B11)</f>
         <v>500</v>
       </c>
-      <c r="C14">
-        <f t="shared" ref="C14:F14" si="1">AVERAGE(C2:C11)</f>
-        <v>1181</v>
+      <c r="C14" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C14:E14" si="1">AVERAGE(D2:D11)</f>
         <v>1840.3</v>
       </c>
       <c r="E14">
@@ -6799,12 +6801,17 @@
         <v>2479.1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
       <c r="B17">
         <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>